<commit_message>
Fixes error with the names of two peptides in the large array
</commit_message>
<xml_diff>
--- a/NASH_serum_data/Reformatted_csvs_2_classes_split_illness/NASH_eighteenR1_repeat_4.xlsx
+++ b/NASH_serum_data/Reformatted_csvs_2_classes_split_illness/NASH_eighteenR1_repeat_4.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CCHept-I17K-L24E</t>
+          <t>CCHept-I17K-I24E</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -2587,7 +2587,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CCHept-L21A</t>
+          <t>CCHept-I24A</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">

</xml_diff>